<commit_message>
TRABAJO FINAL VIERNES 14-11
</commit_message>
<xml_diff>
--- a/backend/app/data/PLANTILLA_VI.xlsx
+++ b/backend/app/data/PLANTILLA_VI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\PROYECTO\PROJECT\FORMATO_VI\vi-app\backend\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492EB86D-9ABC-4719-9736-B03231439726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A083ED-50E4-4568-B316-90247090B8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{3476B835-B212-4DC6-9CBE-82C3B909FDF7}"/>
   </bookViews>
@@ -1122,6 +1122,246 @@
     <xf numFmtId="0" fontId="19" fillId="12" borderId="8" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="4" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="4" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="4" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="4" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="42" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="4" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="6" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="6" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="6" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="6" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="6" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="6" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="6" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="5" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="5" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="5" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="5" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="5" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="7" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="4" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="4" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="10" fillId="4" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1148,246 +1388,6 @@
     </xf>
     <xf numFmtId="4" fontId="10" fillId="4" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="4" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="4" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="4" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="10" fillId="4" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="6" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="6" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="6" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="6" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="6" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="6" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="6" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="5" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="5" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="5" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="5" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="7" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="7" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="7" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="7" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="7" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="7" borderId="22" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="5" borderId="42" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="7" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="7" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="7" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="7" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="7" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="7" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="33" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="34" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="32" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="4" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="4" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="4" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="4" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="9" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="9" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="9" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1403,122 +1403,7 @@
     <cellStyle name="Normal 3 2 8 2" xfId="8" xr:uid="{E139E21A-7616-4B5A-A0FC-BDC6899C50C5}"/>
     <cellStyle name="Porcentaje 2" xfId="10" xr:uid="{592989B5-280D-42B8-A409-6E31379772EA}"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <condense val="0"/>
@@ -2153,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87AFFC31-2662-49F9-BA99-558F38B57518}">
   <dimension ref="A1:BL9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AT4" sqref="AT1:AT1048576"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AU9" sqref="AU8:BL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,52 +2096,52 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
-      <c r="Y1" s="69"/>
-      <c r="Z1" s="69"/>
-      <c r="AA1" s="69"/>
-      <c r="AB1" s="69"/>
-      <c r="AC1" s="69"/>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="69"/>
-      <c r="AF1" s="69"/>
-      <c r="AG1" s="69"/>
-      <c r="AH1" s="69"/>
-      <c r="AI1" s="69"/>
-      <c r="AJ1" s="69"/>
-      <c r="AK1" s="69"/>
-      <c r="AL1" s="69"/>
-      <c r="AM1" s="69"/>
-      <c r="AN1" s="69"/>
-      <c r="AO1" s="70"/>
-      <c r="AP1" s="71" t="s">
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
+      <c r="P1" s="114"/>
+      <c r="Q1" s="114"/>
+      <c r="R1" s="114"/>
+      <c r="S1" s="114"/>
+      <c r="T1" s="114"/>
+      <c r="U1" s="114"/>
+      <c r="V1" s="114"/>
+      <c r="W1" s="114"/>
+      <c r="X1" s="114"/>
+      <c r="Y1" s="114"/>
+      <c r="Z1" s="114"/>
+      <c r="AA1" s="114"/>
+      <c r="AB1" s="114"/>
+      <c r="AC1" s="114"/>
+      <c r="AD1" s="114"/>
+      <c r="AE1" s="114"/>
+      <c r="AF1" s="114"/>
+      <c r="AG1" s="114"/>
+      <c r="AH1" s="114"/>
+      <c r="AI1" s="114"/>
+      <c r="AJ1" s="114"/>
+      <c r="AK1" s="114"/>
+      <c r="AL1" s="114"/>
+      <c r="AM1" s="114"/>
+      <c r="AN1" s="114"/>
+      <c r="AO1" s="115"/>
+      <c r="AP1" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="AQ1" s="72"/>
-      <c r="AR1" s="72"/>
-      <c r="AS1" s="72"/>
-      <c r="AT1" s="73"/>
+      <c r="AQ1" s="117"/>
+      <c r="AR1" s="117"/>
+      <c r="AS1" s="117"/>
+      <c r="AT1" s="118"/>
       <c r="AU1" s="4"/>
       <c r="AV1" s="4"/>
       <c r="AW1" s="4"/>
@@ -2295,52 +2180,52 @@
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="74" t="s">
+      <c r="E2" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="75"/>
-      <c r="AA2" s="75"/>
-      <c r="AB2" s="75"/>
-      <c r="AC2" s="75"/>
-      <c r="AD2" s="75"/>
-      <c r="AE2" s="75"/>
-      <c r="AF2" s="75"/>
-      <c r="AG2" s="75"/>
-      <c r="AH2" s="75"/>
-      <c r="AI2" s="75"/>
-      <c r="AJ2" s="75"/>
-      <c r="AK2" s="75"/>
-      <c r="AL2" s="75"/>
-      <c r="AM2" s="75"/>
-      <c r="AN2" s="75"/>
-      <c r="AO2" s="76"/>
-      <c r="AP2" s="80" t="s">
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="120"/>
+      <c r="O2" s="120"/>
+      <c r="P2" s="120"/>
+      <c r="Q2" s="120"/>
+      <c r="R2" s="120"/>
+      <c r="S2" s="120"/>
+      <c r="T2" s="120"/>
+      <c r="U2" s="120"/>
+      <c r="V2" s="120"/>
+      <c r="W2" s="120"/>
+      <c r="X2" s="120"/>
+      <c r="Y2" s="120"/>
+      <c r="Z2" s="120"/>
+      <c r="AA2" s="120"/>
+      <c r="AB2" s="120"/>
+      <c r="AC2" s="120"/>
+      <c r="AD2" s="120"/>
+      <c r="AE2" s="120"/>
+      <c r="AF2" s="120"/>
+      <c r="AG2" s="120"/>
+      <c r="AH2" s="120"/>
+      <c r="AI2" s="120"/>
+      <c r="AJ2" s="120"/>
+      <c r="AK2" s="120"/>
+      <c r="AL2" s="120"/>
+      <c r="AM2" s="120"/>
+      <c r="AN2" s="120"/>
+      <c r="AO2" s="121"/>
+      <c r="AP2" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="AQ2" s="81"/>
-      <c r="AR2" s="81"/>
-      <c r="AS2" s="81"/>
-      <c r="AT2" s="82"/>
+      <c r="AQ2" s="126"/>
+      <c r="AR2" s="126"/>
+      <c r="AS2" s="126"/>
+      <c r="AT2" s="127"/>
       <c r="AU2" s="4"/>
       <c r="AV2" s="4"/>
       <c r="AW2" s="4"/>
@@ -2375,50 +2260,50 @@
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="18"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78"/>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
-      <c r="U3" s="78"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="78"/>
-      <c r="AB3" s="78"/>
-      <c r="AC3" s="78"/>
-      <c r="AD3" s="78"/>
-      <c r="AE3" s="78"/>
-      <c r="AF3" s="78"/>
-      <c r="AG3" s="78"/>
-      <c r="AH3" s="78"/>
-      <c r="AI3" s="78"/>
-      <c r="AJ3" s="78"/>
-      <c r="AK3" s="78"/>
-      <c r="AL3" s="78"/>
-      <c r="AM3" s="78"/>
-      <c r="AN3" s="78"/>
-      <c r="AO3" s="79"/>
-      <c r="AP3" s="83" t="s">
+      <c r="E3" s="122"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="123"/>
+      <c r="M3" s="123"/>
+      <c r="N3" s="123"/>
+      <c r="O3" s="123"/>
+      <c r="P3" s="123"/>
+      <c r="Q3" s="123"/>
+      <c r="R3" s="123"/>
+      <c r="S3" s="123"/>
+      <c r="T3" s="123"/>
+      <c r="U3" s="123"/>
+      <c r="V3" s="123"/>
+      <c r="W3" s="123"/>
+      <c r="X3" s="123"/>
+      <c r="Y3" s="123"/>
+      <c r="Z3" s="123"/>
+      <c r="AA3" s="123"/>
+      <c r="AB3" s="123"/>
+      <c r="AC3" s="123"/>
+      <c r="AD3" s="123"/>
+      <c r="AE3" s="123"/>
+      <c r="AF3" s="123"/>
+      <c r="AG3" s="123"/>
+      <c r="AH3" s="123"/>
+      <c r="AI3" s="123"/>
+      <c r="AJ3" s="123"/>
+      <c r="AK3" s="123"/>
+      <c r="AL3" s="123"/>
+      <c r="AM3" s="123"/>
+      <c r="AN3" s="123"/>
+      <c r="AO3" s="124"/>
+      <c r="AP3" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="AQ3" s="84"/>
-      <c r="AR3" s="84"/>
-      <c r="AS3" s="84"/>
-      <c r="AT3" s="85"/>
+      <c r="AQ3" s="129"/>
+      <c r="AR3" s="129"/>
+      <c r="AS3" s="129"/>
+      <c r="AT3" s="130"/>
       <c r="AU3" s="4"/>
       <c r="AV3" s="4"/>
       <c r="AW3" s="4"/>
@@ -2439,73 +2324,73 @@
       <c r="BL3" s="11"/>
     </row>
     <row r="4" spans="1:64" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="58">
+      <c r="B4" s="137"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="138">
         <v>2.5</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="59" t="s">
+      <c r="F4" s="138"/>
+      <c r="G4" s="138"/>
+      <c r="H4" s="138"/>
+      <c r="I4" s="138"/>
+      <c r="J4" s="139" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="62">
+      <c r="K4" s="140"/>
+      <c r="L4" s="140"/>
+      <c r="M4" s="140"/>
+      <c r="N4" s="141"/>
+      <c r="O4" s="142">
         <v>160</v>
       </c>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="62"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="63" t="s">
+      <c r="P4" s="142"/>
+      <c r="Q4" s="142"/>
+      <c r="R4" s="142"/>
+      <c r="S4" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
-      <c r="X4" s="64"/>
-      <c r="Y4" s="64"/>
-      <c r="Z4" s="65"/>
+      <c r="T4" s="144"/>
+      <c r="U4" s="144"/>
+      <c r="V4" s="144"/>
+      <c r="W4" s="144"/>
+      <c r="X4" s="144"/>
+      <c r="Y4" s="144"/>
+      <c r="Z4" s="145"/>
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="5"/>
-      <c r="AF4" s="86" t="s">
+      <c r="AF4" s="131" t="s">
         <v>10</v>
       </c>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="87" t="s">
+      <c r="AG4" s="131"/>
+      <c r="AH4" s="132" t="s">
         <v>11</v>
       </c>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="87" t="s">
+      <c r="AI4" s="133"/>
+      <c r="AJ4" s="134"/>
+      <c r="AK4" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="AL4" s="88"/>
-      <c r="AM4" s="89"/>
-      <c r="AN4" s="66" t="s">
+      <c r="AL4" s="133"/>
+      <c r="AM4" s="134"/>
+      <c r="AN4" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="AO4" s="67"/>
-      <c r="AP4" s="90" t="s">
+      <c r="AO4" s="80"/>
+      <c r="AP4" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="AQ4" s="91"/>
-      <c r="AR4" s="66" t="s">
+      <c r="AQ4" s="136"/>
+      <c r="AR4" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="AS4" s="67"/>
+      <c r="AS4" s="80"/>
       <c r="AT4" s="19" t="s">
         <v>14</v>
       </c>
@@ -2529,65 +2414,65 @@
       <c r="BL4" s="11"/>
     </row>
     <row r="5" spans="1:64" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="116"/>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="116"/>
-      <c r="M5" s="116"/>
-      <c r="N5" s="116"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="116"/>
-      <c r="S5" s="116"/>
-      <c r="T5" s="116"/>
-      <c r="U5" s="116"/>
-      <c r="V5" s="116"/>
-      <c r="W5" s="116"/>
-      <c r="X5" s="116"/>
-      <c r="Y5" s="116"/>
-      <c r="Z5" s="117"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="105"/>
+      <c r="N5" s="105"/>
+      <c r="O5" s="105"/>
+      <c r="P5" s="105"/>
+      <c r="Q5" s="105"/>
+      <c r="R5" s="105"/>
+      <c r="S5" s="105"/>
+      <c r="T5" s="105"/>
+      <c r="U5" s="105"/>
+      <c r="V5" s="105"/>
+      <c r="W5" s="105"/>
+      <c r="X5" s="105"/>
+      <c r="Y5" s="105"/>
+      <c r="Z5" s="106"/>
       <c r="AA5" s="20"/>
       <c r="AB5" s="20"/>
       <c r="AC5" s="20"/>
       <c r="AD5" s="20"/>
       <c r="AE5" s="20"/>
-      <c r="AF5" s="118" t="s">
+      <c r="AF5" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AG5" s="118"/>
-      <c r="AH5" s="119" t="s">
+      <c r="AG5" s="107"/>
+      <c r="AH5" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="AI5" s="120"/>
-      <c r="AJ5" s="121"/>
-      <c r="AK5" s="119" t="s">
+      <c r="AI5" s="109"/>
+      <c r="AJ5" s="110"/>
+      <c r="AK5" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="AL5" s="120"/>
-      <c r="AM5" s="121"/>
-      <c r="AN5" s="66" t="s">
+      <c r="AL5" s="109"/>
+      <c r="AM5" s="110"/>
+      <c r="AN5" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="AO5" s="67"/>
-      <c r="AP5" s="122" t="s">
+      <c r="AO5" s="80"/>
+      <c r="AP5" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="AQ5" s="123"/>
-      <c r="AR5" s="66" t="s">
+      <c r="AQ5" s="112"/>
+      <c r="AR5" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="AS5" s="67"/>
+      <c r="AS5" s="80"/>
       <c r="AT5" s="19" t="s">
         <v>14</v>
       </c>
@@ -2611,77 +2496,77 @@
       <c r="BL5" s="11"/>
     </row>
     <row r="6" spans="1:64" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="99" t="s">
+      <c r="D6" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="101" t="s">
+      <c r="E6" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="103" t="s">
+      <c r="F6" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="106" t="s">
+      <c r="G6" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="109" t="s">
+      <c r="H6" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="110"/>
-      <c r="J6" s="113">
+      <c r="I6" s="99"/>
+      <c r="J6" s="102">
         <f>+E4*1000</f>
         <v>2500</v>
       </c>
-      <c r="K6" s="114"/>
-      <c r="L6" s="114"/>
-      <c r="M6" s="114"/>
-      <c r="N6" s="114"/>
-      <c r="O6" s="114"/>
-      <c r="P6" s="114"/>
-      <c r="Q6" s="114"/>
-      <c r="R6" s="114"/>
-      <c r="S6" s="114"/>
-      <c r="T6" s="114"/>
-      <c r="U6" s="115"/>
-      <c r="V6" s="124">
+      <c r="K6" s="103"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="103"/>
+      <c r="S6" s="103"/>
+      <c r="T6" s="103"/>
+      <c r="U6" s="104"/>
+      <c r="V6" s="67">
         <f>AH6*1.6</f>
         <v>25</v>
       </c>
-      <c r="W6" s="125"/>
-      <c r="X6" s="125"/>
-      <c r="Y6" s="125"/>
-      <c r="Z6" s="125"/>
-      <c r="AA6" s="125"/>
-      <c r="AB6" s="125"/>
-      <c r="AC6" s="125"/>
-      <c r="AD6" s="125"/>
-      <c r="AE6" s="125"/>
-      <c r="AF6" s="125"/>
-      <c r="AG6" s="126"/>
-      <c r="AH6" s="124">
+      <c r="W6" s="68"/>
+      <c r="X6" s="68"/>
+      <c r="Y6" s="68"/>
+      <c r="Z6" s="68"/>
+      <c r="AA6" s="68"/>
+      <c r="AB6" s="68"/>
+      <c r="AC6" s="68"/>
+      <c r="AD6" s="68"/>
+      <c r="AE6" s="68"/>
+      <c r="AF6" s="68"/>
+      <c r="AG6" s="69"/>
+      <c r="AH6" s="67">
         <f>J6/O4</f>
         <v>15.625</v>
       </c>
-      <c r="AI6" s="125"/>
-      <c r="AJ6" s="125"/>
-      <c r="AK6" s="125"/>
-      <c r="AL6" s="125"/>
-      <c r="AM6" s="125"/>
-      <c r="AN6" s="125"/>
-      <c r="AO6" s="125"/>
-      <c r="AP6" s="125"/>
-      <c r="AQ6" s="125"/>
-      <c r="AR6" s="125"/>
-      <c r="AS6" s="126"/>
-      <c r="AT6" s="127" t="s">
+      <c r="AI6" s="68"/>
+      <c r="AJ6" s="68"/>
+      <c r="AK6" s="68"/>
+      <c r="AL6" s="68"/>
+      <c r="AM6" s="68"/>
+      <c r="AN6" s="68"/>
+      <c r="AO6" s="68"/>
+      <c r="AP6" s="68"/>
+      <c r="AQ6" s="68"/>
+      <c r="AR6" s="68"/>
+      <c r="AS6" s="69"/>
+      <c r="AT6" s="70" t="s">
         <v>29</v>
       </c>
       <c r="AU6" s="21"/>
@@ -2704,67 +2589,67 @@
       <c r="BL6" s="24"/>
     </row>
     <row r="7" spans="1:64" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="93"/>
-      <c r="B7" s="96"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="107"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="130" t="s">
+      <c r="A7" s="82"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="100"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="131"/>
-      <c r="L7" s="131"/>
-      <c r="M7" s="131"/>
-      <c r="N7" s="131"/>
-      <c r="O7" s="131"/>
-      <c r="P7" s="131"/>
-      <c r="Q7" s="131"/>
-      <c r="R7" s="131"/>
-      <c r="S7" s="131"/>
-      <c r="T7" s="131"/>
-      <c r="U7" s="132"/>
-      <c r="V7" s="133" t="s">
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="75"/>
+      <c r="V7" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="W7" s="134"/>
-      <c r="X7" s="134"/>
-      <c r="Y7" s="134"/>
-      <c r="Z7" s="134"/>
-      <c r="AA7" s="134"/>
-      <c r="AB7" s="134"/>
-      <c r="AC7" s="134"/>
-      <c r="AD7" s="134"/>
-      <c r="AE7" s="134"/>
-      <c r="AF7" s="134"/>
-      <c r="AG7" s="135"/>
-      <c r="AH7" s="133" t="s">
+      <c r="W7" s="77"/>
+      <c r="X7" s="77"/>
+      <c r="Y7" s="77"/>
+      <c r="Z7" s="77"/>
+      <c r="AA7" s="77"/>
+      <c r="AB7" s="77"/>
+      <c r="AC7" s="77"/>
+      <c r="AD7" s="77"/>
+      <c r="AE7" s="77"/>
+      <c r="AF7" s="77"/>
+      <c r="AG7" s="78"/>
+      <c r="AH7" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="AI7" s="134"/>
-      <c r="AJ7" s="134"/>
-      <c r="AK7" s="134"/>
-      <c r="AL7" s="134"/>
-      <c r="AM7" s="134"/>
-      <c r="AN7" s="134"/>
-      <c r="AO7" s="134"/>
-      <c r="AP7" s="134"/>
-      <c r="AQ7" s="134"/>
-      <c r="AR7" s="134"/>
-      <c r="AS7" s="135"/>
-      <c r="AT7" s="128"/>
+      <c r="AI7" s="77"/>
+      <c r="AJ7" s="77"/>
+      <c r="AK7" s="77"/>
+      <c r="AL7" s="77"/>
+      <c r="AM7" s="77"/>
+      <c r="AN7" s="77"/>
+      <c r="AO7" s="77"/>
+      <c r="AP7" s="77"/>
+      <c r="AQ7" s="77"/>
+      <c r="AR7" s="77"/>
+      <c r="AS7" s="78"/>
+      <c r="AT7" s="71"/>
       <c r="AU7" s="21"/>
       <c r="AV7" s="21"/>
       <c r="AW7" s="21"/>
       <c r="AX7" s="21"/>
-      <c r="AY7" s="136" t="s">
+      <c r="AY7" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="AZ7" s="137"/>
-      <c r="BA7" s="138"/>
+      <c r="AZ7" s="58"/>
+      <c r="BA7" s="59"/>
       <c r="BB7" s="23"/>
       <c r="BC7" s="23"/>
       <c r="BD7" s="23"/>
@@ -2778,13 +2663,13 @@
       <c r="BL7" s="24"/>
     </row>
     <row r="8" spans="1:64" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="94"/>
-      <c r="B8" s="96"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="105"/>
-      <c r="G8" s="108"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="97"/>
       <c r="H8" s="28" t="s">
         <v>31</v>
       </c>
@@ -2809,12 +2694,12 @@
       <c r="O8" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="P8" s="139" t="s">
+      <c r="P8" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="Q8" s="140"/>
-      <c r="R8" s="140"/>
-      <c r="S8" s="141"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="61"/>
+      <c r="S8" s="62"/>
       <c r="T8" s="33" t="s">
         <v>10</v>
       </c>
@@ -2839,12 +2724,12 @@
       <c r="AA8" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="AB8" s="142" t="s">
+      <c r="AB8" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="AC8" s="142"/>
-      <c r="AD8" s="142"/>
-      <c r="AE8" s="142"/>
+      <c r="AC8" s="63"/>
+      <c r="AD8" s="63"/>
+      <c r="AE8" s="63"/>
       <c r="AF8" s="33" t="s">
         <v>11</v>
       </c>
@@ -2869,19 +2754,19 @@
       <c r="AM8" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="AN8" s="142" t="s">
+      <c r="AN8" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="AO8" s="142"/>
-      <c r="AP8" s="142"/>
-      <c r="AQ8" s="142"/>
+      <c r="AO8" s="63"/>
+      <c r="AP8" s="63"/>
+      <c r="AQ8" s="63"/>
       <c r="AR8" s="33" t="s">
         <v>12</v>
       </c>
       <c r="AS8" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="AT8" s="129"/>
+      <c r="AT8" s="72"/>
       <c r="AU8" s="23"/>
       <c r="AV8" s="23"/>
       <c r="AW8" s="23"/>
@@ -2897,19 +2782,19 @@
       <c r="BA8" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="BB8" s="143" t="s">
+      <c r="BB8" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="BC8" s="144"/>
-      <c r="BD8" s="144"/>
-      <c r="BE8" s="144"/>
-      <c r="BF8" s="144"/>
-      <c r="BG8" s="144"/>
-      <c r="BH8" s="144"/>
-      <c r="BI8" s="144"/>
-      <c r="BJ8" s="144"/>
-      <c r="BK8" s="144"/>
-      <c r="BL8" s="145"/>
+      <c r="BC8" s="65"/>
+      <c r="BD8" s="65"/>
+      <c r="BE8" s="65"/>
+      <c r="BF8" s="65"/>
+      <c r="BG8" s="65"/>
+      <c r="BH8" s="65"/>
+      <c r="BI8" s="65"/>
+      <c r="BJ8" s="65"/>
+      <c r="BK8" s="65"/>
+      <c r="BL8" s="66"/>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="37">
@@ -3089,17 +2974,22 @@
     <protectedRange sqref="AH9:AN9" name="Rango4"/>
   </protectedRanges>
   <mergeCells count="43">
-    <mergeCell ref="AY7:BA7"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="AB8:AE8"/>
-    <mergeCell ref="AN8:AQ8"/>
-    <mergeCell ref="BB8:BL8"/>
-    <mergeCell ref="V6:AG6"/>
-    <mergeCell ref="AH6:AS6"/>
-    <mergeCell ref="AT6:AT8"/>
-    <mergeCell ref="J7:U7"/>
-    <mergeCell ref="V7:AG7"/>
-    <mergeCell ref="AH7:AS7"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="S4:Z4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="E1:AO1"/>
+    <mergeCell ref="AP1:AT1"/>
+    <mergeCell ref="E2:AO3"/>
+    <mergeCell ref="AP2:AT2"/>
+    <mergeCell ref="AP3:AT3"/>
+    <mergeCell ref="AF4:AG4"/>
+    <mergeCell ref="AH4:AJ4"/>
+    <mergeCell ref="AK4:AM4"/>
+    <mergeCell ref="AN4:AO4"/>
+    <mergeCell ref="AP4:AQ4"/>
     <mergeCell ref="AR5:AS5"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
@@ -3116,22 +3006,17 @@
     <mergeCell ref="AK5:AM5"/>
     <mergeCell ref="AN5:AO5"/>
     <mergeCell ref="AP5:AQ5"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="E1:AO1"/>
-    <mergeCell ref="AP1:AT1"/>
-    <mergeCell ref="E2:AO3"/>
-    <mergeCell ref="AP2:AT2"/>
-    <mergeCell ref="AP3:AT3"/>
-    <mergeCell ref="AF4:AG4"/>
-    <mergeCell ref="AH4:AJ4"/>
-    <mergeCell ref="AK4:AM4"/>
-    <mergeCell ref="AN4:AO4"/>
-    <mergeCell ref="AP4:AQ4"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="S4:Z4"/>
+    <mergeCell ref="V6:AG6"/>
+    <mergeCell ref="AH6:AS6"/>
+    <mergeCell ref="AT6:AT8"/>
+    <mergeCell ref="J7:U7"/>
+    <mergeCell ref="V7:AG7"/>
+    <mergeCell ref="AH7:AS7"/>
+    <mergeCell ref="AY7:BA7"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="AB8:AE8"/>
+    <mergeCell ref="AN8:AQ8"/>
+    <mergeCell ref="BB8:BL8"/>
   </mergeCells>
   <conditionalFormatting sqref="U9 AG9 AS9">
     <cfRule type="cellIs" dxfId="12" priority="19" operator="between">

</xml_diff>